<commit_message>
crud operation for assert management is implemented
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,52 +478,468 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>453</t>
+          <t>A001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>56465</t>
+          <t>Dell Latitude 5420</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>65465</t>
+          <t>Laptop</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>65465</t>
+          <t>2023-01-15</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>65456</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>65465</t>
+          <t>IT Equipment</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>6545</t>
+          <t>Laptop</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>654</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>54565</t>
+          <t>Available</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>47678</t>
+          <t>TechWorld Pvt Ltd</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>A002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>HP ProDesk 400</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Desktop</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2022-11-20</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>55000</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>IT Equipment</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>HP</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Issued</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Global Systems</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>A004</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Projector</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Equipment</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>15-09-2023</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>32000</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Electronics</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Epson</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Vision tech</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>A005</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Lenovo ThinkPad E14</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2023-02-18</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>68000</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>IT Equipment</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Lenovo</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Under Maintenance</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>TechZone</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>A006</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Samsung 27" Monitor</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Monitor</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>2023-03-22</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>22000</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>IT Equipment</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Samsung</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Digital Hub</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>A007</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Canon EOS 1500D</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Camera</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>2022-12-12</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>45000</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Media Equipment</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Canon</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Issued</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Camera World</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>A008</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Logitech MX Master 3</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Mouse</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2023-07-01</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>7500</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Accessories</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Logitech</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Hyderabad</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>TechBazaar</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>A009</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Cisco Catalyst 2960</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Network Switch</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>2022-08-30</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>65000</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Networking</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Cisco</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Issued</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Net Solutions</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>A010</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>MacBook Air M2</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Laptop</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2023-05-14</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>120000</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>IT Equipment</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Apple</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Apple Store</t>
         </is>
       </c>
     </row>
@@ -538,7 +954,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,47 +1012,470 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2543</t>
+          <t>E001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>priya</t>
+          <t>Rahul Sharma</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>development</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>gfghb</t>
+          <t>Software Engineer</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>B+ve</t>
+          <t>B+</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>priya.arunmoli@gmail.com</t>
+          <t>rahul.sharma@company.com</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>3654686765</t>
+          <t>9876543210</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>bangalore</t>
+          <t>Bangalore</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>active</t>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>E002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Priya Nair</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>HR</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>HR Executive</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>O+</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>priya.nair@company.com</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>9876501234</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>E003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Arjun Reddy</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Finance</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Accountant</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>A+</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>arjun.reddy@company.com</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>9876512345</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Hyderabad</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>E004</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Sneha Patel</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Marketing Manager</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>AB+</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>sneha.patel@company.com</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>9876523456</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>E005</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Vikram Singh</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>System Administrator</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>O-</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>vikram.singh@company.com</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>9876534567</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>E006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Anjali Mehta</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Operations</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Operations Executive</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>B-</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>anjali.mehta@company.com</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>9876545678</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Bangalore</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>E007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Karthik Iyer</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Network Engineer</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>A-</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>karthik.iyer@company.com</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>9876556789</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Inactive</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>E008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Meera Joshi</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Sales Executive</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>O+</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>meera.joshi@company.com</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>9876567890</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Hyderabad</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>E009</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Rohit Verma</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Office Administrator</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>B+</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>rohit.verma@company.com</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>9876578901</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>E010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Kavya Rao</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Data Analyst</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>AB-</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>kavya.rao@company.com</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>9876589012</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Pune</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Active</t>
         </is>
       </c>
     </row>
@@ -651,7 +1490,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -711,6 +1550,474 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>T001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>E001</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>A001</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>01-01-2024</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>01-01-2025</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>----</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>IT Manager</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>New laptop issued</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>T002</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>E002</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>A002</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>15-02-2024</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>15-02-2025</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>HR Manager</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Desktop allocated</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>T003</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>E001</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>A001</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>15-02-2024</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>15-02-2025</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>----</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Excellent</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Finance Head</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Official mobile provided</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>T004</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>E004</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>A004</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>05-04-2024</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>05-04-2025</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>----</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Admin Manager</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Printer assigned</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>T005</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>E006</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>A005</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>20-05-2024</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>25-05-2024</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>24-05-2024</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Repaired</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>IT Manager</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Screen replaced</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>T006</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>E007</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>A006</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>12-06-2024</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>12-06-2025</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>----</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Operations Head</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Monitor issued</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>T007</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>E008</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>A008</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Issue</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>01-07-2024</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>01-07-2025</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>----</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>IT Manager</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Network switch allocated</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>T008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>E009</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>A009</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Return</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>15-07-2024</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>15-08-2024</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>10-08-2024</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Sales Manager</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Mouse returned</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>123</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>E005</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>A004</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>qe</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>sd</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>sd</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>sdf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
add.feature of search in chatbot
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -940,6 +940,58 @@
       <c r="J10" t="inlineStr">
         <is>
           <t>Apple Store</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>A1001</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Nil</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>nil</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>12-1-2026</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>7500</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>IT</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Sanz</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>HP</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Available</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Blooms</t>
         </is>
       </c>
     </row>
@@ -1974,7 +2026,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>E005</t>
+          <t>E007</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1984,37 +2036,37 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>qe</t>
+          <t>tfg</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>asd</t>
+          <t>tguj</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>sd</t>
+          <t>ygkj</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>sd</t>
+          <t>hfgh,m</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>sdf</t>
+          <t>jgfjhj,</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>sdf</t>
+          <t>hhjk</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>sdf</t>
+          <t>vbnm</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
formatting in range for asset management system
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1542,7 +1542,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2070,6 +2070,58 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>T010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>E005</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>A004</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>dhj</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>cvbn</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>bdm</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>cdccdcc</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>eeee</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>efcrcrdv</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>ev</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>